<commit_message>
added live or decommisioned
</commit_message>
<xml_diff>
--- a/new.xlsx
+++ b/new.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CompletedProcess(args=['ping', '192.241.152.67'], returncode=0, stdout=b'\r\nPinging 192.241.152.67 with 32 bytes of data:\r\nReply from 192.241.152.67: bytes=32 time=215ms TTL=49\r\nReply from 192.241.152.67: bytes=32 time=215ms TTL=49\r\nReply from 192.241.152.67: bytes=32 time=225ms TTL=49\r\nReply from 192.241.152.67: bytes=32 time=214ms TTL=49\r\n\r\nPing statistics for 192.241.152.67:\r\n    Packets: Sent = 4, Received = 4, Lost = 0 (0% loss),\r\nApproximate round trip times in milli-seconds:\r\n    Minimum = 214ms, Maximum = 225ms, Average = 217ms\r\n', stderr=b'')</t>
+          <t>live</t>
         </is>
       </c>
     </row>
@@ -471,7 +471,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CompletedProcess(args=['ping', '20.102.97.219'], returncode=1, stdout=b'\r\nPinging 20.102.97.219 with 32 bytes of data:\r\nRequest timed out.\r\nRequest timed out.\r\nRequest timed out.\r\nRequest timed out.\r\n\r\nPing statistics for 20.102.97.219:\r\n    Packets: Sent = 4, Received = 0, Lost = 4 (100% loss),\r\n', stderr=b'')</t>
+          <t>decommisioned</t>
         </is>
       </c>
     </row>

</xml_diff>